<commit_message>
Acceptance criteria added for data hydration
</commit_message>
<xml_diff>
--- a/ba_project/data_hydration/User stories template.xlsx
+++ b/ba_project/data_hydration/User stories template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\navin\navin-projects\ba_project\data_hydration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1EA1354-2E8B-42F1-8BC1-7ABC1142C901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF649C2-567C-40FC-A5C9-540F9366F57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -558,8 +558,8 @@
   </sheetPr>
   <dimension ref="A4:Z1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16:G17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>